<commit_message>
Simple Linear Regression Using Excel
</commit_message>
<xml_diff>
--- a/SimpleLinearRegression.xlsx
+++ b/SimpleLinearRegression.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="SLR1" sheetId="1" r:id="rId1"/>
@@ -632,11 +632,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="386393904"/>
-        <c:axId val="386390768"/>
+        <c:axId val="390952312"/>
+        <c:axId val="390948000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="386393904"/>
+        <c:axId val="390952312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -735,12 +735,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386390768"/>
+        <c:crossAx val="390948000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="386390768"/>
+        <c:axId val="390948000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386393904"/>
+        <c:crossAx val="390952312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1279,11 +1279,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="386394688"/>
-        <c:axId val="386391160"/>
+        <c:axId val="390950744"/>
+        <c:axId val="390953880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="386394688"/>
+        <c:axId val="390950744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1329,7 +1329,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1396,12 +1395,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386391160"/>
+        <c:crossAx val="390953880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="386391160"/>
+        <c:axId val="390953880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1446,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1514,7 +1512,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386394688"/>
+        <c:crossAx val="390950744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1611,7 +1609,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1947,11 +1944,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="386388024"/>
-        <c:axId val="386388416"/>
+        <c:axId val="386394688"/>
+        <c:axId val="386392728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="386388024"/>
+        <c:axId val="386394688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,7 +1994,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2064,12 +2060,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386388416"/>
+        <c:crossAx val="386392728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="386388416"/>
+        <c:axId val="386392728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2115,7 +2111,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2182,7 +2177,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386388024"/>
+        <c:crossAx val="386394688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2749,11 +2744,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="384947832"/>
-        <c:axId val="384948224"/>
+        <c:axId val="386391160"/>
+        <c:axId val="386395472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="384947832"/>
+        <c:axId val="386391160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2852,12 +2847,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384948224"/>
+        <c:crossAx val="386395472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="384948224"/>
+        <c:axId val="386395472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2956,7 +2951,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384947832"/>
+        <c:crossAx val="386391160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3045,7 +3040,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3523,11 +3517,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="384949008"/>
-        <c:axId val="124939832"/>
+        <c:axId val="386388024"/>
+        <c:axId val="386388416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="384949008"/>
+        <c:axId val="386388024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3559,7 +3553,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3626,12 +3619,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124939832"/>
+        <c:crossAx val="386388416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124939832"/>
+        <c:axId val="386388416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3663,7 +3656,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3730,7 +3722,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384949008"/>
+        <c:crossAx val="386388024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7013,8 +7005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8341,7 +8333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>

</xml_diff>